<commit_message>
Modified Sprint 3 Backlog for Sprint 3
</commit_message>
<xml_diff>
--- a/sprints/sprint3/Sprint Backlog & Burndown.xlsx
+++ b/sprints/sprint3/Sprint Backlog & Burndown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan Corley\git\SE2-project-repos-sample\sprints\sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0194197c910975a1/Desktop/UWG-SE2-Spring22-Team2/sprints/sprint3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9C4265-351C-41A0-89E5-93A08D9C51A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{9C9C4265-351C-41A0-89E5-93A08D9C51A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F612CD9-90A4-4E69-83B9-1AEE4EB624A1}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Related User Story</t>
   </si>
@@ -64,6 +68,33 @@
   </si>
   <si>
     <t>That User Story</t>
+  </si>
+  <si>
+    <t>I want to be notified when creating an account was successful</t>
+  </si>
+  <si>
+    <t>Modify server side and GUI for account creation success</t>
+  </si>
+  <si>
+    <t>Task Assigned</t>
+  </si>
+  <si>
+    <t>I want to share my pictures to the public</t>
+  </si>
+  <si>
+    <t>I want to share my pictures privately to some users</t>
+  </si>
+  <si>
+    <t>I want to delete images from server side</t>
+  </si>
+  <si>
+    <t>Implement publicly shared functionality</t>
+  </si>
+  <si>
+    <t>Implement privately shared functionality</t>
+  </si>
+  <si>
+    <t>Implement delete functionality for server side</t>
   </si>
 </sst>
 </file>
@@ -145,13 +176,13 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -261,7 +292,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$27:$G$27</c:f>
+              <c:f>Sheet1!$D$27:$H$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1020,13 +1051,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
@@ -1320,314 +1351,360 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.44140625" customWidth="1"/>
+    <col min="2" max="3" width="46.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="7" t="s">
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1">
         <v>100</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>75</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>50</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>25</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
+      <c r="D6" s="1"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
+      <c r="D16" s="1"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="3">
-        <f>SUM(C3:C26)</f>
+      <c r="C27" s="4"/>
+      <c r="D27" s="3">
+        <f>SUM(D3:D26)</f>
         <v>100</v>
       </c>
-      <c r="D27" s="3">
-        <f t="shared" ref="D27:G27" si="0">SUM(D3:D26)</f>
+      <c r="E27" s="3">
+        <f t="shared" ref="E27:H27" si="0">SUM(E3:E26)</f>
         <v>75</v>
       </c>
-      <c r="E27" s="3">
+      <c r="F27" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="F27" s="3">
+      <c r="G27" s="3">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="C1:C2"/>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>